<commit_message>
Updates to design documentation and backlogs
</commit_message>
<xml_diff>
--- a/Planning and Design/SprintProductLog.xlsx
+++ b/Planning and Design/SprintProductLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\recov\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\school_code\CST-247-Project\Planning and Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD3F529-66AF-4760-BCA3-B7D8D7CC9BBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59419D63-6E18-425F-AF1B-A6329FEA67B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26355" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -330,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -365,6 +365,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -378,18 +390,8 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,7 +675,7 @@
   <dimension ref="A1:I2061"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,14 +692,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -706,11 +708,11 @@
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="22"/>
       <c r="G2" s="5"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -751,16 +753,16 @@
       <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="19" t="s">
         <v>36</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="17" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="14"/>
@@ -774,21 +776,25 @@
       <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="18" t="s">
         <v>37</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="17" t="s">
         <v>30</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="7"/>
+      <c r="H5" s="25">
+        <v>44212</v>
+      </c>
+      <c r="I5" s="26">
+        <v>44212</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
@@ -797,21 +803,25 @@
       <c r="B6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="18" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="17" t="s">
         <v>31</v>
       </c>
       <c r="G6" s="14"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="7"/>
+      <c r="H6" s="25">
+        <v>44212</v>
+      </c>
+      <c r="I6" s="26">
+        <v>44212</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -820,16 +830,16 @@
       <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="18" t="s">
         <v>39</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="17" t="s">
         <v>32</v>
       </c>
       <c r="G7" s="14"/>
@@ -843,16 +853,16 @@
       <c r="B8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="18" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="17" t="s">
         <v>33</v>
       </c>
       <c r="G8" s="14"/>
@@ -866,16 +876,16 @@
       <c r="B9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="18" t="s">
         <v>40</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="17" t="s">
         <v>34</v>
       </c>
       <c r="G9" s="14"/>
@@ -889,16 +899,16 @@
       <c r="B10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="18" t="s">
         <v>41</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="17" t="s">
         <v>35</v>
       </c>
       <c r="G10" s="14"/>
@@ -912,16 +922,16 @@
       <c r="B11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="18" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="17" t="s">
         <v>21</v>
       </c>
       <c r="G11" s="14"/>
@@ -23498,15 +23508,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9FDC2B66788A044965A7B8958E6244A" ma:contentTypeVersion="1251" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c2c36359d71eb747fbb188f75fc8d29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="d6188da8-f31e-469a-aed4-03a23c44e36a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="08acee74153637279a480e75df712a71" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -23695,6 +23696,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A856C235-C1E3-486A-AF6F-91B1EB05F3BD}">
   <ds:schemaRefs>
@@ -23706,14 +23716,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C5499EA-2107-4096-9690-EDC799091AC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A347394F-0C4E-4E34-9270-1B2FF1850191}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23730,4 +23732,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C5499EA-2107-4096-9690-EDC799091AC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>